<commit_message>
fixing import asset page
</commit_message>
<xml_diff>
--- a/public/download/SampleImportAsset.xlsx
+++ b/public/download/SampleImportAsset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/MAMP/htdocs/logsheet_php/public/download/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C3A993D-4B0E-BD48-BDB3-8D17714CAC1B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AB22304-53EB-BE47-98A2-74FA7D5F0EE8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="14640" activeTab="1" xr2:uid="{71919B51-AABD-4910-AFC1-52591B11D7AC}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="14640" activeTab="2" xr2:uid="{71919B51-AABD-4910-AFC1-52591B11D7AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Asset" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="104">
   <si>
     <t>Asset Name</t>
   </si>
@@ -140,9 +140,6 @@
     <t>Saturday,Friday</t>
   </si>
   <si>
-    <t>First,Second</t>
-  </si>
-  <si>
     <t>-7.723859129296372','109.00758867445711'</t>
   </si>
   <si>
@@ -218,15 +215,6 @@
     <t>description tekanan</t>
   </si>
   <si>
-    <t>Normal</t>
-  </si>
-  <si>
-    <t>Kurang,Kosong</t>
-  </si>
-  <si>
-    <t>Normal,Kurang,Kosong</t>
-  </si>
-  <si>
     <t>Ada</t>
   </si>
   <si>
@@ -342,15 +330,31 @@
   </si>
   <si>
     <t>Description APAR XX05</t>
+  </si>
+  <si>
+    <t>ms</t>
+  </si>
+  <si>
+    <t>First,Second,Third,Fourth.Last</t>
+  </si>
+  <si>
+    <t>input</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -476,7 +480,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -487,33 +491,33 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -524,34 +528,37 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -868,8 +875,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82EC9F67-5478-4F1C-95CE-25BBFF2D0A56}">
   <dimension ref="A1:U7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -891,49 +898,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="D1" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="27" t="s">
+      <c r="E1" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="24" t="s">
+      <c r="F1" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="24" t="s">
+      <c r="G1" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="24" t="s">
+      <c r="H1" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="24" t="s">
+      <c r="I1" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="24" t="s">
+      <c r="J1" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="24" t="s">
+      <c r="K1" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="24" t="s">
+      <c r="L1" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="M1" s="25" t="s">
+      <c r="M1" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="25" t="s">
+      <c r="N1" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="O1" s="26" t="s">
+      <c r="O1" s="27" t="s">
         <v>16</v>
       </c>
       <c r="P1" s="21"/>
@@ -943,21 +950,21 @@
       <c r="T1" s="22"/>
     </row>
     <row r="2" spans="1:21" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="24"/>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="24"/>
-      <c r="J2" s="24"/>
-      <c r="K2" s="24"/>
-      <c r="L2" s="24"/>
-      <c r="M2" s="25"/>
-      <c r="N2" s="25"/>
-      <c r="O2" s="26"/>
+      <c r="A2" s="25"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
+      <c r="K2" s="25"/>
+      <c r="L2" s="25"/>
+      <c r="M2" s="28"/>
+      <c r="N2" s="28"/>
+      <c r="O2" s="27"/>
       <c r="P2" s="23"/>
       <c r="Q2" s="23"/>
       <c r="R2" s="23"/>
@@ -967,17 +974,17 @@
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>32</v>
@@ -1007,17 +1014,17 @@
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>32</v>
@@ -1035,7 +1042,7 @@
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="N4" s="5"/>
       <c r="O4" s="2" t="s">
@@ -1049,19 +1056,19 @@
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>32</v>
@@ -1074,17 +1081,17 @@
       </c>
       <c r="J5" s="2"/>
       <c r="K5" s="2" t="s">
-        <v>37</v>
+        <v>102</v>
       </c>
       <c r="L5" s="2" t="s">
         <v>36</v>
       </c>
       <c r="M5" s="2"/>
       <c r="N5" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="O5" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="O5" s="2" t="s">
-        <v>39</v>
       </c>
       <c r="P5" s="19"/>
       <c r="Q5" s="19"/>
@@ -1094,17 +1101,17 @@
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>6</v>
@@ -1118,7 +1125,7 @@
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
       <c r="M6" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N6" s="5"/>
       <c r="O6" s="2" t="s">
@@ -1132,19 +1139,19 @@
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="D7" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>43</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>32</v>
@@ -1157,16 +1164,16 @@
       </c>
       <c r="I7" s="2"/>
       <c r="J7" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
       <c r="N7" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="P7" s="19"/>
       <c r="Q7" s="19"/>
@@ -1176,11 +1183,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
     <mergeCell ref="O1:O2"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="G1:G2"/>
@@ -1191,8 +1193,13 @@
     <mergeCell ref="L1:L2"/>
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="N1:N2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
   </mergeCells>
-  <phoneticPr fontId="5" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
@@ -1202,7 +1209,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77A2C89E-7727-9744-BF5A-052E27D4953F}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -1214,76 +1221,76 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="29" t="s">
-        <v>87</v>
-      </c>
-      <c r="B1" s="28" t="s">
-        <v>84</v>
-      </c>
-      <c r="C1" s="28"/>
+      <c r="A1" s="30" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" s="29" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" s="29"/>
     </row>
     <row r="2" spans="1:3" ht="31" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="29"/>
+      <c r="A2" s="30"/>
       <c r="B2" s="16" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="B6" s="2" t="s">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="24" t="s">
+        <v>95</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C6" s="17" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="30" t="s">
-        <v>99</v>
-      </c>
-      <c r="B7" s="2" t="s">
+      <c r="C7" s="3" t="s">
         <v>58</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1299,8 +1306,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{605E4983-905A-5C44-A740-522BEFFC12CF}">
   <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1358,25 +1365,25 @@
         <v>1</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="G2" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="H2" s="9"/>
-      <c r="I2" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="J2" s="9" t="s">
-        <v>29</v>
+        <v>61</v>
+      </c>
+      <c r="D2" s="9">
+        <v>56</v>
+      </c>
+      <c r="E2" s="9">
+        <v>35</v>
+      </c>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="31" t="s">
+        <v>101</v>
+      </c>
+      <c r="I2" s="11"/>
+      <c r="J2" s="31" t="s">
+        <v>103</v>
       </c>
       <c r="K2" s="9" t="s">
         <v>17</v>
@@ -1387,22 +1394,22 @@
         <v>2</v>
       </c>
       <c r="B3" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" s="9" t="s">
         <v>60</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>61</v>
       </c>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
       <c r="F3" s="10" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="H3" s="9"/>
       <c r="I3" s="10" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="J3" s="9" t="s">
         <v>29</v>
@@ -1416,22 +1423,22 @@
         <v>3</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
       <c r="F4" s="11" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="H4" s="11"/>
       <c r="I4" s="11" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="J4" s="9" t="s">
         <v>29</v>
@@ -1445,22 +1452,22 @@
         <v>4</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
       <c r="F5" s="11" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="H5" s="9"/>
       <c r="I5" s="9" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="J5" s="9" t="s">
         <v>29</v>
@@ -1474,22 +1481,22 @@
         <v>5</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D6" s="14"/>
       <c r="E6" s="14"/>
       <c r="F6" s="15" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="G6" s="15" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="H6" s="14"/>
       <c r="I6" s="9" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="J6" s="13" t="s">
         <v>29</v>
@@ -1503,22 +1510,22 @@
         <v>6</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D7" s="14"/>
       <c r="E7" s="14"/>
       <c r="F7" s="15" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="G7" s="15" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="H7" s="14"/>
       <c r="I7" s="9" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="J7" s="13" t="s">
         <v>29</v>
@@ -1532,22 +1539,22 @@
         <v>7</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D8" s="14"/>
       <c r="E8" s="14"/>
       <c r="F8" s="15" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="G8" s="15" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="H8" s="14"/>
       <c r="I8" s="9" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="J8" s="13" t="s">
         <v>29</v>

</xml_diff>